<commit_message>
cleaned up requirement specifications
</commit_message>
<xml_diff>
--- a/Documentation/Krav Specifikation.xlsx
+++ b/Documentation/Krav Specifikation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benjamin\source\repos\Interdisciplinary_Project\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6461D75-1E9C-4FA6-9864-8E4897C6D3FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{033178E5-0DB1-4452-B869-0D94A8014FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="159">
   <si>
     <t>Id</t>
   </si>
@@ -114,12 +114,6 @@
     <t>Specification Pattern data retrievel from context</t>
   </si>
   <si>
-    <t>Can read data from context</t>
-  </si>
-  <si>
-    <t>Can insert data into context</t>
-  </si>
-  <si>
     <t>File Handling</t>
   </si>
   <si>
@@ -294,9 +288,6 @@
     <t>Context-1</t>
   </si>
   <si>
-    <t>Context-2</t>
-  </si>
-  <si>
     <t>End-1</t>
   </si>
   <si>
@@ -508,6 +499,9 @@
   </si>
   <si>
     <t>Factories to create entities, one for each aggregate root</t>
+  </si>
+  <si>
+    <t>Can read and insert data to and from context via backend</t>
   </si>
 </sst>
 </file>
@@ -839,10 +833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,274 +869,268 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" t="s">
         <v>59</v>
       </c>
-      <c r="C5" t="s">
-        <v>61</v>
-      </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="G6" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
         <v>51</v>
       </c>
-      <c r="C8" t="s">
-        <v>53</v>
-      </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>158</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>89</v>
+        <v>154</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>157</v>
+        <v>88</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="2">
-        <v>1</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>159</v>
+      <c r="A13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="1">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>159</v>
+      <c r="A14" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
         <v>44</v>
@@ -1151,825 +1139,814 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>139</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>157</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C20" t="s">
-        <v>142</v>
+        <v>23</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="D21" s="2">
-        <v>1</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F21" s="2"/>
+      <c r="A21" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="B22" t="s">
         <v>32</v>
       </c>
       <c r="C22" t="s">
-        <v>160</v>
+        <v>71</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="F22" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B23" s="2" t="s">
+      <c r="A23" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="2">
-        <v>1</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F23" s="2"/>
+      <c r="C23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B24" s="2" t="s">
+      <c r="A24" t="s">
+        <v>140</v>
+      </c>
+      <c r="B24" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" s="2">
-        <v>1</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F24" s="2"/>
+      <c r="C24" t="s">
+        <v>141</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="2">
-        <v>1</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F25" s="2"/>
+      <c r="A25" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>38</v>
+      </c>
+      <c r="F25" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C26" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="F26" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D27" s="2">
-        <v>1</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F27" s="2"/>
+      <c r="A27" t="s">
+        <v>114</v>
+      </c>
+      <c r="B27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="2">
-        <v>1</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F28" s="2"/>
+      <c r="A28" t="s">
+        <v>118</v>
+      </c>
+      <c r="B28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>38</v>
+      </c>
+      <c r="F28" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D29" s="2">
-        <v>1</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>145</v>
+      <c r="A29" t="s">
+        <v>119</v>
+      </c>
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>38</v>
+      </c>
+      <c r="F29" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="B30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D30">
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="F30" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F31" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C32" t="s">
-        <v>73</v>
+        <v>27</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>40</v>
-      </c>
-      <c r="F32" t="s">
-        <v>137</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="B33" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C33" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="D33">
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>40</v>
-      </c>
-      <c r="F33" t="s">
-        <v>138</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>143</v>
+        <v>75</v>
       </c>
       <c r="B34" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="C34" t="s">
-        <v>144</v>
+        <v>54</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E34" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="F34" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>114</v>
+        <v>76</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C35" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E35" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F35" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>115</v>
+        <v>77</v>
       </c>
       <c r="B36" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="C36" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E36" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F36" t="s">
-        <v>130</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" t="s">
         <v>67</v>
       </c>
-      <c r="C37" t="s">
-        <v>68</v>
-      </c>
       <c r="D37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E37" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F37" t="s">
-        <v>140</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>121</v>
+        <v>87</v>
       </c>
       <c r="B38" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E38" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F38" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
       <c r="B39" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="C39" t="s">
-        <v>21</v>
+        <v>146</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E39" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F39" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>123</v>
+        <v>83</v>
       </c>
       <c r="B40" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="C40" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E40" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F40" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>124</v>
+        <v>91</v>
       </c>
       <c r="B41" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E41" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F41" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B42" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C42" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E42" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="F42" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B43" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C43" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E43" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="F43" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="B44" t="s">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="C44" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="D44">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E44" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F44" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="B45" t="s">
-        <v>63</v>
+        <v>29</v>
       </c>
       <c r="C45" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="D45">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E45" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F45" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>79</v>
+        <v>115</v>
       </c>
       <c r="B46" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C46" t="s">
-        <v>64</v>
+        <v>130</v>
       </c>
       <c r="D46">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E46" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F46" t="s">
-        <v>65</v>
+        <v>126</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="B47" t="s">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="C47" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
       <c r="D47">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E47" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F47" t="s">
-        <v>66</v>
+        <v>126</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="B48" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C48" t="s">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="D48">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E48" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F48" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>84</v>
+        <v>131</v>
       </c>
       <c r="B49" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="C49" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="D49">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E49" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F49" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>85</v>
-      </c>
-      <c r="B50" t="s">
-        <v>51</v>
-      </c>
-      <c r="C50" t="s">
-        <v>58</v>
-      </c>
-      <c r="D50">
-        <v>4</v>
-      </c>
-      <c r="E50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F50" t="s">
-        <v>128</v>
+      <c r="A50" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>94</v>
-      </c>
-      <c r="B51" t="s">
-        <v>41</v>
-      </c>
-      <c r="C51" t="s">
-        <v>49</v>
-      </c>
-      <c r="D51">
-        <v>4</v>
-      </c>
-      <c r="E51" t="s">
-        <v>40</v>
-      </c>
-      <c r="F51" t="s">
-        <v>129</v>
+      <c r="A51" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D51" s="1">
+        <v>9999</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>120</v>
-      </c>
-      <c r="B52" t="s">
-        <v>67</v>
-      </c>
-      <c r="C52" t="s">
-        <v>72</v>
-      </c>
-      <c r="D52">
-        <v>5</v>
-      </c>
-      <c r="E52" t="s">
-        <v>40</v>
-      </c>
-      <c r="F52" t="s">
-        <v>71</v>
-      </c>
+      <c r="A52" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D52" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F52" s="2"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>119</v>
-      </c>
-      <c r="B53" t="s">
-        <v>67</v>
-      </c>
-      <c r="C53" t="s">
-        <v>70</v>
-      </c>
-      <c r="D53">
-        <v>7</v>
-      </c>
-      <c r="E53" t="s">
-        <v>40</v>
-      </c>
-      <c r="F53" t="s">
-        <v>71</v>
-      </c>
+      <c r="A53" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F53" s="2"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>101</v>
-      </c>
-      <c r="B54" t="s">
-        <v>31</v>
-      </c>
-      <c r="C54" t="s">
-        <v>7</v>
-      </c>
-      <c r="D54">
-        <v>8</v>
-      </c>
-      <c r="E54" t="s">
-        <v>40</v>
-      </c>
-      <c r="F54" t="s">
-        <v>129</v>
-      </c>
+      <c r="A54" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D54" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F54" s="2"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="A55" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B55" t="s">
-        <v>31</v>
-      </c>
-      <c r="C55" t="s">
-        <v>8</v>
-      </c>
-      <c r="D55">
-        <v>8</v>
-      </c>
-      <c r="E55" t="s">
-        <v>40</v>
-      </c>
-      <c r="F55" t="s">
-        <v>129</v>
-      </c>
+      <c r="B55" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D55" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F55" s="2"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>118</v>
-      </c>
-      <c r="B56" t="s">
-        <v>67</v>
-      </c>
-      <c r="C56" t="s">
-        <v>133</v>
-      </c>
-      <c r="D56">
-        <v>8</v>
-      </c>
-      <c r="E56" t="s">
-        <v>40</v>
-      </c>
-      <c r="F56" t="s">
-        <v>129</v>
-      </c>
+      <c r="A56" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F56" s="2"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="A57" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B57" t="s">
-        <v>31</v>
-      </c>
-      <c r="C57" t="s">
-        <v>9</v>
-      </c>
-      <c r="D57">
-        <v>9</v>
-      </c>
-      <c r="E57" t="s">
-        <v>40</v>
-      </c>
-      <c r="F57" t="s">
-        <v>129</v>
-      </c>
+      <c r="B57" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F57" s="2"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="A58" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B58" t="s">
-        <v>31</v>
-      </c>
-      <c r="C58" t="s">
-        <v>10</v>
-      </c>
-      <c r="D58">
-        <v>9</v>
-      </c>
-      <c r="E58" t="s">
-        <v>40</v>
-      </c>
-      <c r="F58" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>134</v>
-      </c>
-      <c r="B59" t="s">
-        <v>31</v>
-      </c>
-      <c r="C59" t="s">
-        <v>135</v>
-      </c>
-      <c r="D59">
-        <v>9</v>
-      </c>
-      <c r="E59" t="s">
-        <v>40</v>
-      </c>
-      <c r="F59" t="s">
-        <v>129</v>
+      <c r="B58" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D58" s="2">
+        <v>9999</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated some documentation, fixed an error in a model, and updated test cases
</commit_message>
<xml_diff>
--- a/Documentation/Krav Specifikation.xlsx
+++ b/Documentation/Krav Specifikation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benjamin\source\repos\Interdisciplinary_Project\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85612D9C-381C-46FF-831D-D3C30150C4D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69EB8F9E-6284-49F4-89DD-6A9E1DB9691F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1000,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1578,13 +1578,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D31" s="1">
         <v>1</v>
@@ -1598,13 +1598,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D32" s="1">
         <v>1</v>
@@ -1618,33 +1618,30 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>117</v>
+        <v>158</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>22</v>
+        <v>159</v>
       </c>
       <c r="D33" s="1">
         <v>1</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D34" s="1">
         <v>1</v>
@@ -1655,47 +1652,47 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>33</v>
+        <v>163</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="D35" s="1">
         <v>1</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>38</v>
+        <v>165</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>163</v>
+        <v>33</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="D36" s="1">
         <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>165</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D37" s="1">
         <v>1</v>
@@ -1706,47 +1703,47 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D38" s="1">
         <v>1</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>38</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D39" s="1">
         <v>1</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>165</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D40" s="1">
         <v>1</v>
@@ -1757,13 +1754,13 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D41" s="1">
         <v>1</v>
@@ -1774,13 +1771,13 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D42" s="1">
         <v>1</v>
@@ -1791,50 +1788,50 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>178</v>
+        <v>118</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>179</v>
+        <v>46</v>
       </c>
       <c r="D43" s="1">
         <v>1</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>38</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="D44" s="1">
         <v>1</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>119</v>
+        <v>182</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>27</v>
+        <v>188</v>
       </c>
       <c r="D45" s="1">
         <v>1</v>
@@ -1845,13 +1842,13 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D46" s="1">
         <v>1</v>
@@ -1862,13 +1859,13 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D47" s="1">
         <v>1</v>
@@ -1879,13 +1876,13 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D48" s="1">
         <v>1</v>
@@ -1896,13 +1893,13 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D49" s="1">
         <v>1</v>
@@ -1913,13 +1910,13 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D50" s="1">
         <v>1</v>
@@ -1930,50 +1927,53 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>187</v>
+        <v>120</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>193</v>
+        <v>28</v>
       </c>
       <c r="D51" s="1">
         <v>1</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>38</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>120</v>
+        <v>75</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="D52" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>181</v>
+        <v>123</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D53" s="1">
         <v>2</v>
@@ -1987,13 +1987,13 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D54" s="1">
         <v>2</v>
@@ -2002,18 +2002,18 @@
         <v>38</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>123</v>
+        <v>63</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="D55" s="1">
         <v>2</v>
@@ -2022,58 +2022,58 @@
         <v>38</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="D56" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>64</v>
+        <v>123</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>40</v>
+        <v>143</v>
       </c>
       <c r="D57" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>143</v>
+        <v>56</v>
       </c>
       <c r="D58" s="1">
         <v>4</v>
@@ -2082,18 +2082,18 @@
         <v>38</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D59" s="1">
         <v>4</v>
@@ -2102,41 +2102,41 @@
         <v>38</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>91</v>
+        <v>114</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="D60" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>123</v>
+        <v>69</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>65</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D61" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>38</v>
@@ -2147,33 +2147,33 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>68</v>
+        <v>7</v>
       </c>
       <c r="D62" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>69</v>
+        <v>123</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D63" s="1">
         <v>8</v>
@@ -2187,13 +2187,13 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>29</v>
+        <v>65</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>8</v>
+        <v>127</v>
       </c>
       <c r="D64" s="1">
         <v>8</v>
@@ -2207,16 +2207,16 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>127</v>
+        <v>9</v>
       </c>
       <c r="D65" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>38</v>
@@ -2227,13 +2227,13 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D66" s="1">
         <v>9</v>
@@ -2247,13 +2247,13 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>100</v>
+        <v>128</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="D67" s="1">
         <v>9</v>
@@ -2267,73 +2267,73 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>128</v>
+        <v>150</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>129</v>
+        <v>15</v>
       </c>
       <c r="D68" s="1">
-        <v>9</v>
+        <v>9999</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>38</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>123</v>
+        <v>153</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B69" s="1" t="s">
+      <c r="A69" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D69" s="1">
+      <c r="C69" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D69" s="2">
         <v>9999</v>
       </c>
-      <c r="E69" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F69" s="1" t="s">
+      <c r="E69" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F69" s="2" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D70" s="2">
+      <c r="A70" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D70" s="1">
         <v>9999</v>
       </c>
-      <c r="E70" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>153</v>
+      <c r="E70" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>135</v>
+        <v>17</v>
       </c>
       <c r="D71" s="1">
         <v>9999</v>
@@ -2341,19 +2341,16 @@
       <c r="E71" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F71" s="1" t="s">
-        <v>197</v>
-      </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D72" s="1">
         <v>9999</v>
@@ -2364,13 +2361,13 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D73" s="1">
         <v>9999</v>
@@ -2378,16 +2375,19 @@
       <c r="E73" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="F73" s="1" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D74" s="1">
         <v>9999</v>
@@ -2396,7 +2396,7 @@
         <v>38</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>